<commit_message>
Changes to TitleBlock schematic, Minor BOM fixes
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for TechDemo/REV1/Generate Files/BOM/Bill of Materials-TechDemo.xlsx
+++ b/Hardware/Project Outputs for TechDemo/REV1/Generate Files/BOM/Bill of Materials-TechDemo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="464">
   <si>
     <t xml:space="preserve">Column=LibRef</t>
   </si>
@@ -225,10 +225,10 @@
     <t xml:space="preserve">H. Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">12/12/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6:54 AM</t>
+    <t xml:space="preserve">12/13/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:07 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity</t>
@@ -237,6 +237,18 @@
     <t xml:space="preserve">LibRef</t>
   </si>
   <si>
+    <t xml:space="preserve">CONN_BATTERY_18650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP_2.2UF_50V_0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP_27PF_50V_0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP_4.7PF_50V_0603</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAP_0.1UF_50V_0603</t>
   </si>
   <si>
@@ -246,201 +258,186 @@
     <t xml:space="preserve">CAP_1.0UF_50V_0805</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP_2.2UF_50V_0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP_4.7PF_50V_0603</t>
+    <t xml:space="preserve">CAP_18PF_50V_0805</t>
   </si>
   <si>
     <t xml:space="preserve">CAP_18NF_50V_0805</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP_18PF_50V_0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP_27PF_50V_0603</t>
+    <t xml:space="preserve">DIODE_1N4148W-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE_SCHOTTKY_MBRS2040LT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE_TVS_GSOT03C-G3-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE_ZENER_MMSZ5227BS-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODULE_NHD-4.3-480272EF-ASXV#-CTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITE_BLM21AG102SN1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_6P_SINGLE_ROW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_HIROSE_DM3BT-DSF-PEJS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_MOLEX_0512964033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_MOLEX_0522070660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_USB_MOLEX_0475900001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_3P_SINGLE_ROW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_TD_EXPANSION_MODULE</t>
   </si>
   <si>
     <t xml:space="preserve">CONN_2P_SINGLE_ROW</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN_3P_SINGLE_ROW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_6P_SINGLE_ROW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_BATTERY_18650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_HIROSE_DM3BT-DSF-PEJS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_MOLEX_0512964033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_MOLEX_0522070660</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_TD_EXPANSION_MODULE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_USB_MOLEX_0475900001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE_1N4148W-7-F</t>
+    <t xml:space="preserve">INDUCTOR_LPS4018-472MRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUCTOR_SDR0403-1R0ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUCTOR_IHLP2020BZER1R0M01</t>
   </si>
   <si>
     <t xml:space="preserve">DIODE_LED_GREEN_LTST-C170GKT</t>
   </si>
   <si>
-    <t xml:space="preserve">DIODE_SCHOTTKY_MBRS2040LT3G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE_TVS_GSOT03C-G3-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE_ZENER_MMSZ5227BS-7-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRITE_BLM21AG102SN1D</t>
+    <t xml:space="preserve">LED_RED_GREEN_HSMF-A201-A00J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET_PCH_IRLML5103PBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET_NCH_2N7002-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET_PCH_NTR3A30PZT1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_200_0805_1/8W_1%_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_1M_0603_1/10W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_10K_0603_1/10W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_100K_0603_1/10W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_0_0805_1/8W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_10K_0805_1/4W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_100K_0805_1/4W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_5.1_0805_1/4W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_15K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_1K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_120_0805_1/4W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_POT_10K_500mW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_0.140_1206_1/4W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_768K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_137K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_40.2K_0805_1/8W_1%_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_402K_0805_1/8W_1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_DIP_220ADC16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCH_EVQ-Q2U02W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_STM32F746NGH6U</t>
   </si>
   <si>
     <t xml:space="preserve">IC_ IS42S32400F-6TL</t>
   </si>
   <si>
+    <t xml:space="preserve">IC_MT25QL128ABA1ESE-0SIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_TPS61169DCKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_RCLAMP0504FATCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_STMPS2141MTR</t>
+  </si>
+  <si>
     <t xml:space="preserve">IC_LIS3DHTR</t>
   </si>
   <si>
+    <t xml:space="preserve">MODULE_RCWL-1601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_TPL0401A-10DCKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_OPAMP_TSV620ILT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_OPAMP_LM4861</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_NX3DV221TKX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODULE_WRL-1746</t>
+  </si>
+  <si>
     <t xml:space="preserve">IC_MCP73826-4.1VCHTR</t>
   </si>
   <si>
-    <t xml:space="preserve">IC_MT25QL128ABA1ESE-0SIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_NX3DV221TKX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_OPAMP_LM4861</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_OPAMP_TSV620ILT</t>
+    <t xml:space="preserve">IC_TPS63020DSJR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC_TPS61230DRCR</t>
   </si>
   <si>
     <t xml:space="preserve">IC_OSC_ECS-2520MVLC-250-BN-TR</t>
   </si>
   <si>
-    <t xml:space="preserve">IC_RCLAMP0504FATCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_STM32F746NGH6U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_STMPS2141MTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_TPL0401A-10DCKR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_TPS61169DCKR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_TPS61230DRCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC_TPS63020DSJR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUCTOR_IHLP2020BZER1R0M01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUCTOR_LPS4018-472MRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUCTOR_SDR0403-1R0ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED_RED_GREEN_HSMF-A201-A00J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MODULE_NHD-4.3-480272EF-ASXV#-CTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MODULE_RCWL-1601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MODULE_WRL-1746</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET_NCH_2N7002-7-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET_PCH_IRLML5103PBF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET_PCH_NTR3A30PZT1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_0_0805_1/8W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_0.140_1206_1/4W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_1K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_1M_0603_1/10W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_5.1_0805_1/4W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_10K_0603_1/10W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_10K_0805_1/4W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_10K_0805_1/4W_1%_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_15K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_40.2K_0805_1/8W_1%_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_100K_0603_1/10W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_100K_0805_1/4W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_120_0805_1/4W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_137K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_200_0805_1/8W_1%_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_402K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_768K_0805_1/8W_1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES_POT_10K_500mW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW_DIP_220ADC16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SWITCH_EVQ-Q2U02W</t>
-  </si>
-  <si>
     <t xml:space="preserve">XTAL_25HZ_6PF_SMD</t>
   </si>
   <si>
@@ -450,6 +447,15 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">BATTERY CONTACT CLP 18650 PC PIN (NOTE: QTY x2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 2.2UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 4.7PF 50V C0G/NPO 0603</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAP CER 0.1UF 50V X7R 0603</t>
   </si>
   <si>
@@ -459,189 +465,183 @@
     <t xml:space="preserve">CAP CER 1UF 50V X7R 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP CER 2.2UF 50V X7R 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 4.7PF 50V C0G/NPO 0603</t>
+    <t xml:space="preserve">CAP CER 18PF 50V C0G/NP0 0805</t>
   </si>
   <si>
     <t xml:space="preserve">CAP CER 0.018UF 50V X7R 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP CER 18PF 50V C0G/NP0 0805</t>
+    <t xml:space="preserve">DIODE GEN PURP 100V 300MA SOD123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE SCHOTTKY 40V 2A SMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVS DIODE 3.3V 12.3V SOT23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE ZENER 3.6V 200MW SOD323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD TFT 480X272 HIGH BRIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITE, 1KOHM AT 100MHZ, 220MA, .450DCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 6POS 2.54MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN MICRO SD CARD PUSH-PUSH R/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN FFC BOTTOM 40POS 0.50MM R/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN FPC TOP 6POS 1.00MM R/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN RCPT MICRO USB AB 5P SMD RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 3POS 2.54MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 5POS 2.54MM (NOTE: QTY x4)</t>
   </si>
   <si>
     <t xml:space="preserve">CONN HEADER VERT 2POS 2.54MM</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN HEADER VERT 3POS 2.54MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN HEADER VERT 6POS 2.54MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BATTERY CONTACT CLP 18650 PC PIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN MICRO SD CARD PUSH-PUSH R/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN FFC BOTTOM 40POS 0.50MM R/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN FPC TOP 6POS 1.00MM R/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN RCPT MICRO USB AB 5P SMD RA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE GEN PURP 100V 300MA SOD123</t>
+    <t xml:space="preserve">SHIELDED POWER INDUCTORS, 4.7UH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXED IND 1UH 3.8A 33 MOHM SMD</t>
   </si>
   <si>
     <t xml:space="preserve">DIODE, LED GREEN CLEAR SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">DIODE SCHOTTKY 40V 2A SMB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVS DIODE 3.3V 12.3V SOT23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE ZENER 3.6V 200MW SOD323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRITE, 1KOHM AT 100MHZ, 220MA, .450DCR</t>
+    <t xml:space="preserve">LED GREEN/RED CLEAR 4PLCC SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET P CHN, VDS=30V, RDSON = .6OHM, SOT 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET N-CH 60V 115MA SOT23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET P-CH 20V 3A SOT23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 200 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 1M OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 0 OHM JUMPER 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 10K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 100K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 5.1 OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 15K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 120 OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIMMER 10K OHM 0.5W PC PIN TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 0.14 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 768K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 137K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 40.2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 402K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCH ROTARY DIP HEX 100MA 50V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCH TACTILE SPST-NO 0.02A 15V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F746NGH6 (STM32F7 Birdie) TBGA216</t>
   </si>
   <si>
     <t xml:space="preserve">IC DRAM 128M PARALLEL 86TSOP II</t>
   </si>
   <si>
+    <t xml:space="preserve">IC FLASH 128M SPI 133MHZ 8SOP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC LED DRVR RGLTR DIM 1.8A SC70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVS DIODE 5V 25V SC70-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC PWR SWITCH N-CHANNEL 1:1 8SO</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACCEL 2-16G I2C/SPI 16LGA</t>
   </si>
   <si>
+    <t xml:space="preserve">MODULE ULTRASONIC SENSOR 3V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC DGTL POT 10KOHM 128TAP SC70-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC OPAMP GP 1 CIRCUIT SOT23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC AMP CLASS AB MONO 1.5W 8SOIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC USB 2.0 SWITCH HS 10HVSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIFI MODULE - ESP8266 4MB FLASH</t>
+  </si>
+  <si>
     <t xml:space="preserve">IC CONTROLLR LI-ION 4.1V SOT23-6</t>
   </si>
   <si>
-    <t xml:space="preserve">IC FLASH 128M SPI 133MHZ 8SOP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC USB 2.0 SWITCH HS 10HVSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC AMP CLASS AB MONO 1.5W 8SOIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC OPAMP GP 1 CIRCUIT SOT23-6</t>
+    <t xml:space="preserve">IC REG BCK BST ADJ 3.5A 14VSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG BOOST ADJ 4A 10VSON</t>
   </si>
   <si>
     <t xml:space="preserve">XTAL OSC XO 25MHZ CMOS SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">TVS DIODE 5V 25V SC70-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F746NGH6 (STM32F7 Birdie) TBGA216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC PWR SWITCH N-CHANNEL 1:1 8SO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC DGTL POT 10KOHM 128TAP SC70-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC LED DRVR RGLTR DIM 1.8A SC70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC REG BOOST ADJ 4A 10VSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC REG BCK BST ADJ 3.5A 14VSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIXED IND 1UH 3.8A 33 MOHM SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIELDED POWER INDUCTORS, 4.7UH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED GREEN/RED CLEAR 4PLCC SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCD TFT 480X272 HIGH BRIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MODULE ULTRASONIC SENSOR 3V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIFI MODULE - ESP8266 4MB FLASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET N-CH 60V 115MA SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET P CHN, VDS=30V, RDSON = .6OHM, SOT 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET P-CH 20V 3A SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 0 OHM JUMPER 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES 0.14 OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 1K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 1M OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES 5.1 OHM 1% 1/4W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 10K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 10K OHM 1% 1/4W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 15K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 40.2K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 100K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 100K OHM 1% 1/4W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES 120 OHM 1% 1/4W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 137K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 200 OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 402K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 768K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRIMMER 10K OHM 0.5W PC PIN TOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SWITCH ROTARY DIP HEX 100MA 50V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SWITCH TACTILE SPST-NO 0.02A 15V</t>
-  </si>
-  <si>
     <t xml:space="preserve">CRYSTAL 25.0000MHZ 18PF SMD</t>
   </si>
   <si>
@@ -651,6 +651,18 @@
     <t xml:space="preserve">Designator</t>
   </si>
   <si>
+    <t xml:space="preserve">BAT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C22, C23, C24, C25, C26, C27, C28, C29, C54, C61, C62, C63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2, C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4, C5</t>
+  </si>
+  <si>
     <t xml:space="preserve">C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C32, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43</t>
   </si>
   <si>
@@ -660,204 +672,189 @@
     <t xml:space="preserve">C46, C55</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C22, C23, C24, C25, C26, C27, C28, C29, C54, C61, C62, C63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4, C5</t>
+    <t xml:space="preserve">C72</t>
   </si>
   <si>
     <t xml:space="preserve">C73</t>
   </si>
   <si>
-    <t xml:space="preserve">C72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2, C3</t>
+    <t xml:space="preserve">D1, D5, D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2, D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3, D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1, FB2, FB3, FB4, FB5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J7, J11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J8</t>
   </si>
   <si>
     <t xml:space="preserve">J9, J10, J12, J13</t>
   </si>
   <si>
-    <t xml:space="preserve">J7, J11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1, D5, D6</t>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3</t>
   </si>
   <si>
     <t xml:space="preserve">LED1</t>
   </si>
   <si>
-    <t xml:space="preserve">D2, D7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3, D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB1, FB2, FB3, FB4, FB5</t>
+    <t xml:space="preserve">LED2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2, Q3, Q4, Q5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q6, Q7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R5, R34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6, R7, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R67, R68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8, R29, R30, R55, R56, R59, R60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9, R45, R47, R49, R52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27, R35, R36, R37, R40, R41, R42, R43, R46, R48, R50, R51, R53, R61, R64, R65, R66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R31, R32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R38, R39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
   </si>
   <si>
     <t xml:space="preserve">U2</t>
   </si>
   <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
     <t xml:space="preserve">U7</t>
   </si>
   <si>
+    <t xml:space="preserve">U8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U13</t>
+  </si>
+  <si>
     <t xml:space="preserve">U14</t>
   </si>
   <si>
-    <t xml:space="preserve">U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10</t>
+    <t xml:space="preserve">U15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U16</t>
   </si>
   <si>
     <t xml:space="preserve">X1</t>
   </si>
   <si>
-    <t xml:space="preserve">U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2, Q3, Q4, Q5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q6, Q7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8, R29, R30, R55, R56, R59, R60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2, R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R5, R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R45, R47, R49, R52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R31, R32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6, R7, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R67, R68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R27, R35, R36, R37, R40, R41, R42, R43, R46, R48, R50, R51, R53, R61, R64, R65, R66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R38, R39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW2</t>
-  </si>
-  <si>
     <t xml:space="preserve">X2</t>
   </si>
   <si>
@@ -867,108 +864,120 @@
     <t xml:space="preserve">MFG</t>
   </si>
   <si>
+    <t xml:space="preserve">Keystone Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiyo Yuden</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yageo</t>
   </si>
   <si>
     <t xml:space="preserve">AVX</t>
   </si>
   <si>
-    <t xml:space="preserve">Taiyo Yuden</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stackpole Electronics Inc</t>
   </si>
   <si>
+    <t xml:space="preserve">Diodes Incorporated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newhaven Display Intl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MURATA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sullins Connector Solutions</t>
   </si>
   <si>
-    <t xml:space="preserve">Keystone Electronics</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hirose Electric Co Ltd</t>
   </si>
   <si>
     <t xml:space="preserve">Molex</t>
   </si>
   <si>
-    <t xml:space="preserve">Diodes Incorporated</t>
+    <t xml:space="preserve">COILCRAFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bourns Inc.</t>
   </si>
   <si>
     <t xml:space="preserve">Lite-On Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">ON SEMICONDUCTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Semiconductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MURATA</t>
+    <t xml:space="preserve">Broadcom Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERNATIONAL RECTIFIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOA Speer Electronics, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTS Electrocomponents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMicroelectronics</t>
   </si>
   <si>
     <t xml:space="preserve">ISSI, Integrated Silicon Solution Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">STMicroelectronics</t>
+    <t xml:space="preserve">Micron Technology Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semtech Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit Industries LLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXP USA Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparkfun</t>
   </si>
   <si>
     <t xml:space="preserve">Microchip Technology</t>
   </si>
   <si>
-    <t xml:space="preserve">Micron Technology Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NXP USA Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
     <t xml:space="preserve">ECS Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">Semtech Corporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bourns Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COILCRAFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Broadcom Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Newhaven Display Intl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adafruit Industries LLC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sparkfun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTERNATIONAL RECTIFIER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ON Semiconductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOA Speer Electronics, Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTS Electrocomponents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panasonic Electronic Components</t>
-  </si>
-  <si>
     <t xml:space="preserve">EPSON</t>
   </si>
   <si>
     <t xml:space="preserve">MFG_PN</t>
   </si>
   <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMK212BB7225MG-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603KRNPO9BN270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603CRNPO9BN4R7</t>
+  </si>
+  <si>
     <t xml:space="preserve">CC0603KRX7R9BB104</t>
   </si>
   <si>
@@ -978,198 +987,186 @@
     <t xml:space="preserve">UMK212B7105MGHT</t>
   </si>
   <si>
-    <t xml:space="preserve">UMK212BB7225MG-T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603CRNPO9BN4R7</t>
+    <t xml:space="preserve">CML0805C0G180JT50V</t>
   </si>
   <si>
     <t xml:space="preserve">CC0805KRX7R9BB183</t>
   </si>
   <si>
-    <t xml:space="preserve">CML0805C0G180JT50V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603KRNPO9BN270</t>
+    <t xml:space="preserve">1N4148W-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBRS2040LT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSOT03C-G3-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMSZ5227BS-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHD-4.3-480272EF-ASXV#-CTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLM21AG102SN1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREC006SFAN-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM3BT-DSF-PEJS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0512964033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0522070660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0475900001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREC003SFAN-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPTC051LFBN-RC</t>
   </si>
   <si>
     <t xml:space="preserve">PREC002SFAN-RC</t>
   </si>
   <si>
-    <t xml:space="preserve">PREC003SFAN-RC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PREC006SFAN-RC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM3BT-DSF-PEJS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0512964033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0522070660</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPTC151LFBN-RC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0475900001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1N4148W-7-F</t>
+    <t xml:space="preserve">LPS4018-472MRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDR0403-1R0ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IHLP2020BZER1R0M01</t>
   </si>
   <si>
     <t xml:space="preserve">LTST-C170GKT</t>
   </si>
   <si>
-    <t xml:space="preserve">MBRS2040LT3G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSOT03C-G3-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMSZ5227BS-7-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLM21AG102SN1D</t>
+    <t xml:space="preserve">HSMF-A201-A00J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRLML5103PBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2N7002-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTR3A30PZT1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07200RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-071ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805JR-070RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG73S2ATTD1002F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK73H2ATTD1003F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK73H2ATTD5R10F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-0715KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-071KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK73H2ATTD1200F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3386F-1-103TLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RL1206FR-070R14L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07768KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07137KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-0740K2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07402KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220ADC16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVQ-Q2U02W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F746IGT6</t>
   </si>
   <si>
     <t xml:space="preserve">IS42S32400F-6TL-TR</t>
   </si>
   <si>
+    <t xml:space="preserve">MT25QL128ABA1ESE-0SIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS61169DCKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCLAMP0504FATCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMPS2141MTR</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIS3DHTR</t>
   </si>
   <si>
+    <t xml:space="preserve">4007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPL0401A-10DCKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSV620ILT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM4861MX/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NX3DV221TKX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WRL-17146</t>
+  </si>
+  <si>
     <t xml:space="preserve">MCP73826-4.1VCHTR</t>
   </si>
   <si>
-    <t xml:space="preserve">MT25QL128ABA1ESE-0SIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NX3DV221TKX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LM4861MX/NOPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSV620ILT</t>
+    <t xml:space="preserve">TPS63020DSJR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS61230DRCR</t>
   </si>
   <si>
     <t xml:space="preserve">ECS-2520MVLC-250-BN-TR</t>
   </si>
   <si>
-    <t xml:space="preserve">RCLAMP0504FATCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F746IGT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STMPS2141MTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPL0401A-10DCKR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPS61169DCKR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPS61230DRCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPS63020DSJR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IHLP2020BZER1R0M01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPS4018-472MRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDR0403-1R0ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSMF-A201-A00J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHD-4.3-480272EF-ASXV#-CTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WRL-17146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2N7002-7-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRLML5103PBF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTR3A30PZT1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805JR-070RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RL1206FR-070R14L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-071KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-071ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK73H2ATTD5R10F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG73S2ATTD1002F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-0715KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-0740K2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-07100KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK73H2ATTD1003F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK73H2ATTD1200F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-07137KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-07200RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-07402KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-07768KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3386F-1-103TLF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220ADC16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EVQ-Q2U02W</t>
-  </si>
-  <si>
     <t xml:space="preserve">ECS-250-18-7SX-TR</t>
   </si>
   <si>
@@ -1182,15 +1179,27 @@
     <t xml:space="preserve">Digi-Key</t>
   </si>
   <si>
+    <t xml:space="preserve">DigiKey</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mouser</t>
   </si>
   <si>
-    <t xml:space="preserve">DigiKey</t>
-  </si>
-  <si>
     <t xml:space="preserve">Supplier Part Number 1</t>
   </si>
   <si>
+    <t xml:space="preserve">36-54-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587-4963-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-4032-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1740-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">311-1344-1-ND</t>
   </si>
   <si>
@@ -1200,192 +1209,180 @@
     <t xml:space="preserve">587-6375-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">587-4963-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-1740-1-ND</t>
+    <t xml:space="preserve">738-CML0805C0G180JT50VCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">311-1137-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">738-CML0805C0G180JT50VCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-4032-1-ND</t>
+    <t xml:space="preserve">1N4148W-FDICT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBRS2040LT3GOSCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSOT03C-G3-08GICT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMSZ5227BS-FDICT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHD-4.3-480272EF-ASXV#-CTP-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-1041-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1212EC-06-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR1942CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM11237CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM10939CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM17144CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1212EC-03-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6103-ND</t>
   </si>
   <si>
     <t xml:space="preserve">S1212EC-02-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">S1212EC-03-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S1212EC-06-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36-54-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR1942CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM11237CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM10939CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S7013-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM17144CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1N4148W-FDICT-ND</t>
+    <t xml:space="preserve">2457-LPS4018-472MRC-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDR0403-1R0MLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">541-1087-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">160-1179-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">MBRS2040LT3GOSCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSOT03C-G3-08GICT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMSZ5227BS-FDICT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-1041-1-ND</t>
+    <t xml:space="preserve">516-2491-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRLML5103PBFCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2N7002-FDICT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTR3A30PZT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-200CRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1.00MHRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-0.0ARCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-SG73S2ATTD1002FCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-RK73H2ATTD1003FCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-RK73H2ATTD5R10FCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-15.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1.00KCRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-RK73H2ATTD1200FCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3386F-103TLF-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-.14LWCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-768KCRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-137KCRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-40.2KCRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-402KCRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT3070-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P12954SCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-15817-ND</t>
   </si>
   <si>
     <t xml:space="preserve">870-IS42S32400F-6TL</t>
   </si>
   <si>
+    <t xml:space="preserve">557-1772-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-40821-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCLAMP0504FATCTCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-6932-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">497-10613-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">1528-2832-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-29676-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-10160-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-38566-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">568-10368-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">MCP73826-4.1VCHCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">557-1772-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">568-10368-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-38566-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">497-10160-1-ND</t>
+    <t xml:space="preserve">296-36491-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-37761-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">50-ECS-2520MVLC-250-BN-CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">RCLAMP0504FATCTCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">497-15817-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">497-6932-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-29676-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-40821-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-37761-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-36491-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541-1087-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2457-LPS4018-472MRC-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDR0403-1R0MLCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">516-2491-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHD-4.3-480272EF-ASXV#-CTP-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1528-2832-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2N7002-FDICT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRLML5103PBFCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTR3A30PZT1GOSCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-0.0ARCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-.14LWCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-1.00KCRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-1.00MHRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-RK73H2ATTD5R10FCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-10.0KHRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-SG73S2ATTD1002FCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-15.0KCRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-40.2KCRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-RK73H2ATTD1003FCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-RK73H2ATTD1200FCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-137KCRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-200CRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-402KCRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-768KCRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3386F-103TLF-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT3070-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P12954SCT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">XC2030-1-ND</t>
   </si>
   <si>
@@ -1404,7 +1401,7 @@
     <t xml:space="preserve">195</t>
   </si>
   <si>
-    <t xml:space="preserve">12/12/2020 6:54 AM</t>
+    <t xml:space="preserve">12/13/2020 8:07 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Bill of Materials</t>
@@ -2863,11 +2860,11 @@
       </c>
       <c r="E8" s="41">
         <f ca="1">TODAY()</f>
-        <v>44177</v>
+        <v>44178</v>
       </c>
       <c r="F8" s="42">
         <f ca="1">NOW()</f>
-        <v>44177.2875163912</v>
+        <v>44178.3385404494</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="39"/>
@@ -2890,25 +2887,25 @@
         <v>69</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>207</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>57</v>
@@ -2924,28 +2921,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="60">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D10" s="55" t="s">
         <v>70</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" s="58" t="s">
         <v>208</v>
       </c>
       <c r="G10" s="58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H10" s="58" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I10" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J10" s="58" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K10" s="69"/>
       <c r="L10" s="70">
@@ -2962,32 +2959,32 @@
         <v>2</v>
       </c>
       <c r="C11" s="61">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11" s="56" t="s">
         <v>71</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>209</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H11" s="56" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I11" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J11" s="56" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K11" s="71"/>
       <c r="L11" s="74">
-        <f t="shared" ref="L11:L80" si="0">C11*K11</f>
+        <f t="shared" ref="L11:L79" si="0">C11*K11</f>
         <v>0</v>
       </c>
       <c r="M11"/>
@@ -3006,22 +3003,22 @@
         <v>72</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F12" s="58" t="s">
         <v>210</v>
       </c>
       <c r="G12" s="58" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H12" s="58" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I12" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J12" s="58" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K12" s="69"/>
       <c r="L12" s="70">
@@ -3038,28 +3035,28 @@
         <v>4</v>
       </c>
       <c r="C13" s="61">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D13" s="56" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>211</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H13" s="56" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I13" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K13" s="71"/>
       <c r="L13" s="74">
@@ -3076,28 +3073,28 @@
         <v>5</v>
       </c>
       <c r="C14" s="60">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D14" s="55" t="s">
         <v>74</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F14" s="58" t="s">
         <v>212</v>
       </c>
       <c r="G14" s="58" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H14" s="58" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I14" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J14" s="58" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K14" s="69"/>
       <c r="L14" s="70">
@@ -3114,28 +3111,28 @@
         <v>6</v>
       </c>
       <c r="C15" s="61">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D15" s="56" t="s">
         <v>75</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F15" s="56" t="s">
         <v>213</v>
       </c>
       <c r="G15" s="56" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H15" s="56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I15" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J15" s="56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K15" s="71"/>
       <c r="L15" s="74">
@@ -3152,28 +3149,28 @@
         <v>7</v>
       </c>
       <c r="C16" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="55" t="s">
         <v>76</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" s="58" t="s">
         <v>214</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I16" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J16" s="58" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K16" s="69"/>
       <c r="L16" s="70">
@@ -3190,28 +3187,28 @@
         <v>8</v>
       </c>
       <c r="C17" s="61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="56" t="s">
         <v>77</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F17" s="56" t="s">
         <v>215</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="H17" s="56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I17" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K17" s="71"/>
       <c r="L17" s="74">
@@ -3228,28 +3225,28 @@
         <v>9</v>
       </c>
       <c r="C18" s="60">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="55" t="s">
         <v>78</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F18" s="58" t="s">
         <v>216</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H18" s="58" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I18" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J18" s="58" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K18" s="69"/>
       <c r="L18" s="70">
@@ -3266,13 +3263,13 @@
         <v>10</v>
       </c>
       <c r="C19" s="61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="56" t="s">
         <v>79</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" s="56" t="s">
         <v>217</v>
@@ -3281,13 +3278,13 @@
         <v>284</v>
       </c>
       <c r="H19" s="56" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I19" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J19" s="56" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K19" s="71"/>
       <c r="L19" s="74">
@@ -3304,28 +3301,28 @@
         <v>11</v>
       </c>
       <c r="C20" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="55" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F20" s="58" t="s">
         <v>218</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H20" s="58" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I20" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J20" s="58" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K20" s="69"/>
       <c r="L20" s="70">
@@ -3342,28 +3339,28 @@
         <v>12</v>
       </c>
       <c r="C21" s="61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="56" t="s">
         <v>81</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F21" s="56" t="s">
         <v>219</v>
       </c>
       <c r="G21" s="56" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H21" s="56" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I21" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J21" s="56" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K21" s="71"/>
       <c r="L21" s="74">
@@ -3386,7 +3383,7 @@
         <v>82</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F22" s="58" t="s">
         <v>220</v>
@@ -3395,13 +3392,13 @@
         <v>286</v>
       </c>
       <c r="H22" s="58" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I22" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J22" s="58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K22" s="69"/>
       <c r="L22" s="70">
@@ -3424,7 +3421,7 @@
         <v>83</v>
       </c>
       <c r="E23" s="56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F23" s="56" t="s">
         <v>221</v>
@@ -3433,13 +3430,13 @@
         <v>287</v>
       </c>
       <c r="H23" s="56" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I23" s="56" t="s">
         <v>384</v>
       </c>
       <c r="J23" s="56" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K23" s="71"/>
       <c r="L23" s="74">
@@ -3456,28 +3453,28 @@
         <v>15</v>
       </c>
       <c r="C24" s="60">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D24" s="55" t="s">
         <v>84</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F24" s="58" t="s">
         <v>222</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H24" s="58" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I24" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J24" s="58" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K24" s="69"/>
       <c r="L24" s="70">
@@ -3500,22 +3497,22 @@
         <v>85</v>
       </c>
       <c r="E25" s="56" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F25" s="56" t="s">
         <v>223</v>
       </c>
       <c r="G25" s="56" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="H25" s="56" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I25" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J25" s="56" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K25" s="71"/>
       <c r="L25" s="74">
@@ -3544,16 +3541,16 @@
         <v>224</v>
       </c>
       <c r="G26" s="58" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H26" s="58" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I26" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J26" s="58" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K26" s="69"/>
       <c r="L26" s="70">
@@ -3570,7 +3567,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" s="56" t="s">
         <v>87</v>
@@ -3582,16 +3579,16 @@
         <v>225</v>
       </c>
       <c r="G27" s="56" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H27" s="56" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I27" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J27" s="56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K27" s="71"/>
       <c r="L27" s="74">
@@ -3620,16 +3617,16 @@
         <v>226</v>
       </c>
       <c r="G28" s="58" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H28" s="58" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I28" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J28" s="58" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K28" s="69"/>
       <c r="L28" s="70">
@@ -3646,7 +3643,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="56" t="s">
         <v>89</v>
@@ -3658,16 +3655,16 @@
         <v>227</v>
       </c>
       <c r="G29" s="56" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H29" s="56" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I29" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J29" s="56" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K29" s="71"/>
       <c r="L29" s="74">
@@ -3696,16 +3693,16 @@
         <v>228</v>
       </c>
       <c r="G30" s="58" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H30" s="58" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I30" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J30" s="58" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K30" s="69"/>
       <c r="L30" s="70">
@@ -3734,16 +3731,16 @@
         <v>229</v>
       </c>
       <c r="G31" s="56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H31" s="56" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I31" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J31" s="56" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K31" s="71"/>
       <c r="L31" s="74">
@@ -3760,7 +3757,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="55" t="s">
         <v>92</v>
@@ -3772,16 +3769,16 @@
         <v>230</v>
       </c>
       <c r="G32" s="58" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H32" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I32" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J32" s="58" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K32" s="69"/>
       <c r="L32" s="70">
@@ -3810,16 +3807,16 @@
         <v>231</v>
       </c>
       <c r="G33" s="56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H33" s="56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I33" s="56" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J33" s="56" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K33" s="71"/>
       <c r="L33" s="74">
@@ -3848,16 +3845,16 @@
         <v>232</v>
       </c>
       <c r="G34" s="58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H34" s="58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I34" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J34" s="58" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K34" s="69"/>
       <c r="L34" s="70">
@@ -3880,22 +3877,22 @@
         <v>95</v>
       </c>
       <c r="E35" s="56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F35" s="56" t="s">
         <v>233</v>
       </c>
       <c r="G35" s="56" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H35" s="56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I35" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J35" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K35" s="71"/>
       <c r="L35" s="74">
@@ -3918,22 +3915,22 @@
         <v>96</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F36" s="58" t="s">
         <v>234</v>
       </c>
       <c r="G36" s="58" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H36" s="58" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I36" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J36" s="58" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K36" s="69"/>
       <c r="L36" s="70">
@@ -3956,22 +3953,22 @@
         <v>97</v>
       </c>
       <c r="E37" s="56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F37" s="56" t="s">
         <v>235</v>
       </c>
       <c r="G37" s="56" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H37" s="56" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I37" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J37" s="56" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K37" s="71"/>
       <c r="L37" s="74">
@@ -3994,22 +3991,22 @@
         <v>98</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F38" s="58" t="s">
         <v>236</v>
       </c>
       <c r="G38" s="58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H38" s="58" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I38" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J38" s="58" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K38" s="69"/>
       <c r="L38" s="70">
@@ -4026,28 +4023,28 @@
         <v>30</v>
       </c>
       <c r="C39" s="61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D39" s="56" t="s">
         <v>99</v>
       </c>
       <c r="E39" s="56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F39" s="56" t="s">
         <v>237</v>
       </c>
       <c r="G39" s="56" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="H39" s="56" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I39" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J39" s="56" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K39" s="71"/>
       <c r="L39" s="74">
@@ -4064,28 +4061,28 @@
         <v>31</v>
       </c>
       <c r="C40" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="55" t="s">
         <v>100</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F40" s="58" t="s">
         <v>238</v>
       </c>
       <c r="G40" s="58" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H40" s="58" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I40" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J40" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K40" s="69"/>
       <c r="L40" s="70">
@@ -4108,22 +4105,22 @@
         <v>101</v>
       </c>
       <c r="E41" s="56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F41" s="56" t="s">
         <v>239</v>
       </c>
       <c r="G41" s="56" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="H41" s="56" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I41" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J41" s="56" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K41" s="71"/>
       <c r="L41" s="74">
@@ -4140,28 +4137,28 @@
         <v>33</v>
       </c>
       <c r="C42" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" s="55" t="s">
         <v>102</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F42" s="58" t="s">
         <v>240</v>
       </c>
       <c r="G42" s="58" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="H42" s="58" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I42" s="58" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J42" s="58" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K42" s="69"/>
       <c r="L42" s="70">
@@ -4178,28 +4175,28 @@
         <v>34</v>
       </c>
       <c r="C43" s="61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" s="56" t="s">
         <v>103</v>
       </c>
       <c r="E43" s="56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F43" s="56" t="s">
         <v>241</v>
       </c>
       <c r="G43" s="56" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="H43" s="56" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I43" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J43" s="56" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K43" s="71"/>
       <c r="L43" s="74">
@@ -4216,28 +4213,28 @@
         <v>35</v>
       </c>
       <c r="C44" s="60">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D44" s="55" t="s">
         <v>104</v>
       </c>
       <c r="E44" s="55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F44" s="58" t="s">
         <v>242</v>
       </c>
       <c r="G44" s="58" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="H44" s="58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I44" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J44" s="58" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K44" s="69"/>
       <c r="L44" s="70">
@@ -4254,28 +4251,28 @@
         <v>36</v>
       </c>
       <c r="C45" s="61">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D45" s="56" t="s">
         <v>105</v>
       </c>
       <c r="E45" s="56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F45" s="56" t="s">
         <v>243</v>
       </c>
       <c r="G45" s="56" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="H45" s="56" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I45" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J45" s="56" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="K45" s="71"/>
       <c r="L45" s="74">
@@ -4292,13 +4289,13 @@
         <v>37</v>
       </c>
       <c r="C46" s="60">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D46" s="55" t="s">
         <v>106</v>
       </c>
       <c r="E46" s="55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F46" s="58" t="s">
         <v>244</v>
@@ -4307,13 +4304,13 @@
         <v>298</v>
       </c>
       <c r="H46" s="58" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I46" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J46" s="58" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="K46" s="69"/>
       <c r="L46" s="70">
@@ -4333,10 +4330,10 @@
         <v>1</v>
       </c>
       <c r="D47" s="56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E47" s="56" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F47" s="56" t="s">
         <v>245</v>
@@ -4345,13 +4342,13 @@
         <v>298</v>
       </c>
       <c r="H47" s="56" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I47" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J47" s="56" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="K47" s="71"/>
       <c r="L47" s="74">
@@ -4368,28 +4365,28 @@
         <v>39</v>
       </c>
       <c r="C48" s="60">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D48" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E48" s="55" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F48" s="58" t="s">
         <v>246</v>
       </c>
       <c r="G48" s="58" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H48" s="58" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I48" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J48" s="58" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="K48" s="69"/>
       <c r="L48" s="70">
@@ -4409,25 +4406,25 @@
         <v>1</v>
       </c>
       <c r="D49" s="56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E49" s="56" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F49" s="56" t="s">
         <v>247</v>
       </c>
       <c r="G49" s="56" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H49" s="56" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I49" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J49" s="56" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="K49" s="71"/>
       <c r="L49" s="74">
@@ -4444,10 +4441,10 @@
         <v>41</v>
       </c>
       <c r="C50" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" s="55" t="s">
         <v>177</v>
@@ -4456,16 +4453,16 @@
         <v>248</v>
       </c>
       <c r="G50" s="58" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="H50" s="58" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I50" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J50" s="58" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="K50" s="69"/>
       <c r="L50" s="70">
@@ -4485,25 +4482,25 @@
         <v>1</v>
       </c>
       <c r="D51" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E51" s="56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F51" s="56" t="s">
         <v>249</v>
       </c>
       <c r="G51" s="56" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
       <c r="H51" s="56" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I51" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J51" s="56" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="K51" s="71"/>
       <c r="L51" s="74">
@@ -4520,28 +4517,28 @@
         <v>43</v>
       </c>
       <c r="C52" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E52" s="55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F52" s="58" t="s">
         <v>250</v>
       </c>
       <c r="G52" s="58" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H52" s="58" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I52" s="58" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J52" s="58" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="K52" s="69"/>
       <c r="L52" s="70">
@@ -4561,25 +4558,25 @@
         <v>1</v>
       </c>
       <c r="D53" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E53" s="56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F53" s="56" t="s">
         <v>251</v>
       </c>
       <c r="G53" s="56" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="H53" s="56" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I53" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J53" s="56" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="K53" s="71"/>
       <c r="L53" s="74">
@@ -4599,24 +4596,26 @@
         <v>1</v>
       </c>
       <c r="D54" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E54" s="55" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F54" s="58" t="s">
         <v>252</v>
       </c>
       <c r="G54" s="58" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
       <c r="H54" s="58" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I54" s="58" t="s">
-        <v>384</v>
-      </c>
-      <c r="J54" s="58"/>
+        <v>383</v>
+      </c>
+      <c r="J54" s="58" t="s">
+        <v>429</v>
+      </c>
       <c r="K54" s="69"/>
       <c r="L54" s="70">
         <f>C54*K54</f>
@@ -4632,28 +4631,28 @@
         <v>46</v>
       </c>
       <c r="C55" s="61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D55" s="56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E55" s="56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F55" s="56" t="s">
         <v>253</v>
       </c>
       <c r="G55" s="56" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="H55" s="56" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="I55" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J55" s="56" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K55" s="71"/>
       <c r="L55" s="74">
@@ -4673,25 +4672,25 @@
         <v>1</v>
       </c>
       <c r="D56" s="55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E56" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F56" s="58" t="s">
         <v>254</v>
       </c>
       <c r="G56" s="58" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="H56" s="58" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I56" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J56" s="58" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K56" s="69"/>
       <c r="L56" s="70">
@@ -4708,28 +4707,28 @@
         <v>48</v>
       </c>
       <c r="C57" s="61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" s="56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E57" s="56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F57" s="56" t="s">
         <v>255</v>
       </c>
       <c r="G57" s="56" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="H57" s="56" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I57" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J57" s="56" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="K57" s="71"/>
       <c r="L57" s="74">
@@ -4746,28 +4745,28 @@
         <v>49</v>
       </c>
       <c r="C58" s="60">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D58" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E58" s="55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F58" s="58" t="s">
         <v>256</v>
       </c>
       <c r="G58" s="58" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H58" s="58" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I58" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J58" s="58" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K58" s="69"/>
       <c r="L58" s="70">
@@ -4787,25 +4786,25 @@
         <v>1</v>
       </c>
       <c r="D59" s="56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E59" s="56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F59" s="56" t="s">
         <v>257</v>
       </c>
       <c r="G59" s="56" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="H59" s="56" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I59" s="56" t="s">
         <v>384</v>
       </c>
       <c r="J59" s="56" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K59" s="71"/>
       <c r="L59" s="74">
@@ -4825,25 +4824,25 @@
         <v>1</v>
       </c>
       <c r="D60" s="55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E60" s="55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F60" s="58" t="s">
         <v>258</v>
       </c>
       <c r="G60" s="58" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="H60" s="58" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I60" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J60" s="58" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K60" s="69"/>
       <c r="L60" s="70">
@@ -4860,28 +4859,28 @@
         <v>52</v>
       </c>
       <c r="C61" s="61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E61" s="56" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F61" s="56" t="s">
         <v>259</v>
       </c>
       <c r="G61" s="56" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="H61" s="56" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I61" s="56" t="s">
         <v>384</v>
       </c>
       <c r="J61" s="56" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K61" s="71"/>
       <c r="L61" s="74">
@@ -4901,25 +4900,25 @@
         <v>1</v>
       </c>
       <c r="D62" s="55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E62" s="55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F62" s="58" t="s">
         <v>260</v>
       </c>
       <c r="G62" s="58" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="H62" s="58" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I62" s="58" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J62" s="58" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="K62" s="69"/>
       <c r="L62" s="70">
@@ -4936,28 +4935,28 @@
         <v>54</v>
       </c>
       <c r="C63" s="61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D63" s="56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E63" s="56" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F63" s="56" t="s">
         <v>261</v>
       </c>
       <c r="G63" s="56" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="H63" s="56" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I63" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J63" s="56" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="K63" s="71"/>
       <c r="L63" s="74">
@@ -4977,25 +4976,25 @@
         <v>1</v>
       </c>
       <c r="D64" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E64" s="55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F64" s="58" t="s">
         <v>262</v>
       </c>
       <c r="G64" s="58" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H64" s="58" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I64" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J64" s="58" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K64" s="69"/>
       <c r="L64" s="70">
@@ -5012,7 +5011,7 @@
         <v>56</v>
       </c>
       <c r="C65" s="61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D65" s="56" t="s">
         <v>124</v>
@@ -5024,16 +5023,16 @@
         <v>263</v>
       </c>
       <c r="G65" s="56" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="H65" s="56" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I65" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J65" s="56" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K65" s="71"/>
       <c r="L65" s="74">
@@ -5056,22 +5055,22 @@
         <v>125</v>
       </c>
       <c r="E66" s="55" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F66" s="58" t="s">
         <v>264</v>
       </c>
       <c r="G66" s="58" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="H66" s="58" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="I66" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J66" s="58" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="K66" s="69"/>
       <c r="L66" s="70">
@@ -5088,25 +5087,25 @@
         <v>58</v>
       </c>
       <c r="C67" s="61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="56" t="s">
         <v>126</v>
       </c>
       <c r="E67" s="56" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F67" s="56" t="s">
         <v>265</v>
       </c>
       <c r="G67" s="56" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="H67" s="56" t="s">
         <v>369</v>
       </c>
       <c r="I67" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J67" s="56" t="s">
         <v>442</v>
@@ -5132,19 +5131,19 @@
         <v>127</v>
       </c>
       <c r="E68" s="55" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F68" s="58" t="s">
         <v>266</v>
       </c>
       <c r="G68" s="58" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H68" s="58" t="s">
         <v>370</v>
       </c>
       <c r="I68" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J68" s="58" t="s">
         <v>443</v>
@@ -5164,28 +5163,28 @@
         <v>60</v>
       </c>
       <c r="C69" s="61">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D69" s="56" t="s">
         <v>128</v>
       </c>
       <c r="E69" s="56" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F69" s="56" t="s">
         <v>267</v>
       </c>
       <c r="G69" s="56" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="H69" s="56" t="s">
         <v>371</v>
       </c>
       <c r="I69" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J69" s="56" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="K69" s="71"/>
       <c r="L69" s="74">
@@ -5202,28 +5201,28 @@
         <v>61</v>
       </c>
       <c r="C70" s="60">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D70" s="55" t="s">
         <v>129</v>
       </c>
       <c r="E70" s="55" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F70" s="58" t="s">
         <v>268</v>
       </c>
       <c r="G70" s="58" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H70" s="58" t="s">
         <v>372</v>
       </c>
       <c r="I70" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J70" s="58" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K70" s="69"/>
       <c r="L70" s="70">
@@ -5240,28 +5239,28 @@
         <v>62</v>
       </c>
       <c r="C71" s="61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" s="56" t="s">
         <v>130</v>
       </c>
       <c r="E71" s="56" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F71" s="56" t="s">
         <v>269</v>
       </c>
       <c r="G71" s="56" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H71" s="56" t="s">
         <v>373</v>
       </c>
       <c r="I71" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J71" s="56" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="K71" s="71"/>
       <c r="L71" s="74">
@@ -5284,22 +5283,22 @@
         <v>131</v>
       </c>
       <c r="E72" s="55" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F72" s="58" t="s">
         <v>270</v>
       </c>
       <c r="G72" s="58" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
       <c r="H72" s="58" t="s">
         <v>374</v>
       </c>
       <c r="I72" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J72" s="58" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="K72" s="69"/>
       <c r="L72" s="70">
@@ -5322,23 +5321,21 @@
         <v>132</v>
       </c>
       <c r="E73" s="56" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F73" s="56" t="s">
         <v>271</v>
       </c>
       <c r="G73" s="56" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="H73" s="56" t="s">
         <v>375</v>
       </c>
       <c r="I73" s="56" t="s">
-        <v>384</v>
-      </c>
-      <c r="J73" s="56" t="s">
-        <v>447</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="J73" s="56"/>
       <c r="K73" s="71"/>
       <c r="L73" s="74">
         <f>C73*K73</f>
@@ -5360,19 +5357,19 @@
         <v>133</v>
       </c>
       <c r="E74" s="55" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F74" s="58" t="s">
         <v>272</v>
       </c>
       <c r="G74" s="58" t="s">
-        <v>280</v>
+        <v>309</v>
       </c>
       <c r="H74" s="58" t="s">
         <v>376</v>
       </c>
       <c r="I74" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J74" s="58" t="s">
         <v>448</v>
@@ -5398,19 +5395,19 @@
         <v>134</v>
       </c>
       <c r="E75" s="56" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F75" s="56" t="s">
         <v>273</v>
       </c>
       <c r="G75" s="56" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="H75" s="56" t="s">
         <v>377</v>
       </c>
       <c r="I75" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J75" s="56" t="s">
         <v>449</v>
@@ -5436,19 +5433,19 @@
         <v>135</v>
       </c>
       <c r="E76" s="55" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F76" s="58" t="s">
         <v>274</v>
       </c>
       <c r="G76" s="58" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H76" s="58" t="s">
         <v>378</v>
       </c>
       <c r="I76" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J76" s="58" t="s">
         <v>450</v>
@@ -5474,7 +5471,7 @@
         <v>136</v>
       </c>
       <c r="E77" s="56" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F77" s="56" t="s">
         <v>275</v>
@@ -5486,7 +5483,7 @@
         <v>379</v>
       </c>
       <c r="I77" s="56" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J77" s="56" t="s">
         <v>451</v>
@@ -5512,19 +5509,19 @@
         <v>137</v>
       </c>
       <c r="E78" s="55" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F78" s="58" t="s">
         <v>276</v>
       </c>
       <c r="G78" s="58" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H78" s="58" t="s">
         <v>380</v>
       </c>
       <c r="I78" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J78" s="58" t="s">
         <v>452</v>
@@ -5537,7 +5534,7 @@
       <c r="M78"/>
       <c r="N78"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:13" s="3" customFormat="1" thickBot="1">
       <c r="A79" s="15"/>
       <c r="B79" s="54">
         <f>ROW(B79)-ROW($B$9)</f>
@@ -5550,19 +5547,19 @@
         <v>138</v>
       </c>
       <c r="E79" s="56" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F79" s="56" t="s">
         <v>277</v>
       </c>
       <c r="G79" s="56" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="H79" s="56" t="s">
         <v>381</v>
       </c>
       <c r="I79" s="56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J79" s="56" t="s">
         <v>453</v>
@@ -5575,39 +5572,26 @@
       <c r="M79"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:13" s="3" customFormat="1" thickBot="1">
+    <row r="80" spans="1:13">
       <c r="A80" s="15"/>
-      <c r="B80" s="53">
-        <f>ROW(B80)-ROW($B$9)</f>
-        <v>71</v>
-      </c>
-      <c r="C80" s="60">
-        <v>1</v>
-      </c>
-      <c r="D80" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="E80" s="55" t="s">
-        <v>206</v>
-      </c>
-      <c r="F80" s="58" t="s">
-        <v>278</v>
-      </c>
-      <c r="G80" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="H80" s="58" t="s">
-        <v>382</v>
-      </c>
-      <c r="I80" s="58" t="s">
-        <v>384</v>
-      </c>
-      <c r="J80" s="58" t="s">
-        <v>454</v>
-      </c>
-      <c r="K80" s="69"/>
-      <c r="L80" s="70">
-        <f>C80*K80</f>
+      <c r="B80" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="76"/>
+      <c r="D80" s="76"/>
+      <c r="E80" s="52"/>
+      <c r="F80" s="51"/>
+      <c r="G80" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="K80" s="68"/>
+      <c r="L80" s="73">
+        <f>SUM(L10:L79)</f>
         <v>0</v>
       </c>
       <c r="M80"/>
@@ -5615,26 +5599,17 @@
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="15"/>
-      <c r="B81" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="C81" s="76"/>
-      <c r="D81" s="76"/>
-      <c r="E81" s="52"/>
-      <c r="F81" s="51"/>
-      <c r="G81" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H81"/>
-      <c r="I81"/>
-      <c r="J81" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="K81" s="68"/>
-      <c r="L81" s="73">
-        <f>SUM(L10:L80)</f>
-        <v>0</v>
-      </c>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="20"/>
       <c r="M81"/>
       <c r="N81"/>
     </row>
@@ -5643,14 +5618,14 @@
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="9"/>
-      <c r="L82" s="20"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="21"/>
       <c r="M82"/>
       <c r="N82"/>
     </row>
@@ -5664,45 +5639,36 @@
       <c r="G83" s="10"/>
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
-      <c r="J83" s="10"/>
+      <c r="J83" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="K83" s="10"/>
       <c r="L83" s="21"/>
       <c r="M83"/>
       <c r="N83"/>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:12" thickBot="1">
       <c r="A84" s="15"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="10"/>
-      <c r="H84" s="10"/>
-      <c r="I84" s="10"/>
-      <c r="J84" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K84" s="10"/>
-      <c r="L84" s="21"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="17"/>
+      <c r="K84" s="17"/>
+      <c r="L84" s="22"/>
       <c r="M84"/>
       <c r="N84"/>
     </row>
-    <row r="85" spans="1:12" thickBot="1">
-      <c r="A85" s="15"/>
-      <c r="B85" s="49"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="17"/>
-      <c r="L85" s="22"/>
-      <c r="M85"/>
-      <c r="N85"/>
+    <row r="86" spans="1:12">
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86"/>
+      <c r="H86"/>
     </row>
     <row r="87" spans="1:12">
       <c r="D87" s="1"/>
@@ -5718,16 +5684,9 @@
       <c r="G88"/>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:12">
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89"/>
-      <c r="H89"/>
-    </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B80:D80"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.46" right="0.36" top="0.58" bottom="1" header="0.5" footer="0.5"/>
@@ -5757,7 +5716,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -5797,7 +5756,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -5807,7 +5766,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -5817,7 +5776,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -5847,7 +5806,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -5857,7 +5816,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -5867,7 +5826,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -5877,7 +5836,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -5887,7 +5846,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -5897,7 +5856,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -5907,7 +5866,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>

</xml_diff>

<commit_message>
Fixed U10 footprint, added outline Tsilk J1 Added footprint checkplots
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for TechDemo/REV1/Generate Files/BOM/Bill of Materials-TechDemo.xlsx
+++ b/Hardware/Project Outputs for TechDemo/REV1/Generate Files/BOM/Bill of Materials-TechDemo.xlsx
@@ -225,10 +225,10 @@
     <t xml:space="preserve">H. Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">12/18/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:59 PM</t>
+    <t xml:space="preserve">12/20/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:17 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity</t>
@@ -1470,7 +1470,7 @@
     <t xml:space="preserve">210</t>
   </si>
   <si>
-    <t xml:space="preserve">12/18/2020 9:59 PM</t>
+    <t xml:space="preserve">12/20/2020 1:17 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Bill of Materials</t>
@@ -2929,11 +2929,11 @@
       </c>
       <c r="E8" s="41">
         <f ca="1">TODAY()</f>
-        <v>44183</v>
+        <v>44185</v>
       </c>
       <c r="F8" s="42">
         <f ca="1">NOW()</f>
-        <v>44183.9159794312</v>
+        <v>44185.5538014675</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="39"/>

</xml_diff>

<commit_message>
Major Commit: Test Hardware Firmware This commit adds the firmware to test hardware - all of the major components are working.  0-9 and A-E total tests are added.
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for TechDemo/REV1/Generate Files/BOM/Bill of Materials-TechDemo.xlsx
+++ b/Hardware/Project Outputs for TechDemo/REV1/Generate Files/BOM/Bill of Materials-TechDemo.xlsx
@@ -225,10 +225,10 @@
     <t xml:space="preserve">H. Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">12/20/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:17 PM</t>
+    <t xml:space="preserve">12/23/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:19 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity</t>
@@ -1470,7 +1470,7 @@
     <t xml:space="preserve">210</t>
   </si>
   <si>
-    <t xml:space="preserve">12/20/2020 1:17 PM</t>
+    <t xml:space="preserve">12/23/2020 8:19 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Bill of Materials</t>
@@ -2929,11 +2929,11 @@
       </c>
       <c r="E8" s="41">
         <f ca="1">TODAY()</f>
-        <v>44185</v>
+        <v>44188</v>
       </c>
       <c r="F8" s="42">
         <f ca="1">NOW()</f>
-        <v>44185.5538014675</v>
+        <v>44188.3466157138</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="39"/>

</xml_diff>